<commit_message>
Added support for generating export files for Subtype Group definitions
</commit_message>
<xml_diff>
--- a/TestExcel/Test3.xlsx
+++ b/TestExcel/Test3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -73,15 +73,21 @@
     <t>Id</t>
   </si>
   <si>
-    <t>CustomerName</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
+    <t>CustomerFirstName</t>
+  </si>
+  <si>
+    <t>Customer First Name</t>
   </si>
   <si>
     <t>Character(20)</t>
   </si>
   <si>
+    <t>CustomerLastName</t>
+  </si>
+  <si>
+    <t>Customer Last Name</t>
+  </si>
+  <si>
     <t>CustomerDateTime</t>
   </si>
   <si>
@@ -89,6 +95,12 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>Customer Birthday</t>
+  </si>
+  <si>
+    <t>Birthday</t>
   </si>
   <si>
     <t>Address</t>
@@ -172,7 +184,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,7 +193,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -196,35 +214,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -241,26 +259,26 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -277,43 +295,43 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -333,6 +351,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
     </indexedColors>
@@ -533,17 +552,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -571,10 +590,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -822,12 +841,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1114,7 +1133,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1142,10 +1161,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1396,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1554,156 +1573,156 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" t="s" s="4">
-        <v>21</v>
-      </c>
-      <c r="L6" t="s" s="4">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s" s="4">
-        <v>0</v>
-      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="6">
+      <c r="A7" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="B7" t="s" s="6">
+      <c r="B7" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="C7" s="3"/>
+      <c r="D7" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="8">
+      <c r="A8" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" t="s" s="10">
+      <c r="C8" s="7"/>
+      <c r="D8" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="5">
-        <v>1</v>
-      </c>
+      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" t="s" s="4">
+        <v>28</v>
+      </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="M8" t="s" s="4">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="12">
-        <v>28</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" t="s" s="12">
-        <v>17</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="3"/>
+      <c r="A9" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
       <c r="I9" s="3"/>
-      <c r="J9" t="s" s="4">
-        <v>19</v>
-      </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E10" s="7"/>
+      <c r="A10" t="s" s="12">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" t="s" s="4">
+        <v>19</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="D11" s="14">
-        <v>2</v>
-      </c>
-      <c r="E11" s="14">
-        <v>1</v>
-      </c>
-      <c r="F11" s="11"/>
+      <c r="A11" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="5">
-        <v>2</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="12">
+      <c r="A12" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s" s="10">
         <v>31</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" t="s" s="12">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s" s="12">
-        <v>32</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="14">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="5">
+        <v>2</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="E13" s="7"/>
+      <c r="A13" t="s" s="12">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s" s="12">
+        <v>36</v>
+      </c>
+      <c r="E13" s="13"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1714,22 +1733,18 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="D14" s="14">
-        <v>3</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
+      <c r="A14" t="s" s="6">
+        <v>37</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="5">
-        <v>3</v>
-      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1737,20 +1752,22 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="12">
-        <v>36</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" t="s" s="12">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s" s="12">
-        <v>37</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="3"/>
+      <c r="A15" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="D15" s="14">
+        <v>3</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="5">
+        <v>3</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1758,15 +1775,17 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="4">
-        <v>38</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" t="s" s="4">
-        <v>39</v>
-      </c>
-      <c r="E16" s="3"/>
+      <c r="A16" t="s" s="12">
+        <v>40</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s" s="12">
+        <v>41</v>
+      </c>
+      <c r="E16" s="13"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1778,26 +1797,45 @@
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" t="s" s="4">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s" s="4">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" t="s" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" t="s" s="4">
+        <v>46</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Allow setting length and decimals information in separate columns for domain definitions
</commit_message>
<xml_diff>
--- a/TestExcel/Test3.xlsx
+++ b/TestExcel/Test3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -67,7 +67,7 @@
     <t>PK</t>
   </si>
   <si>
-    <t>Numeric(8.2)</t>
+    <t>Numeric</t>
   </si>
   <si>
     <t>Id</t>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>FeatureId</t>
-  </si>
-  <si>
-    <t>Numeric</t>
   </si>
   <si>
     <t>FeatureName</t>
@@ -1542,7 +1539,9 @@
       <c r="D5" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="5">
+        <v>8.199999999999999</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" t="b" s="5">
         <v>1</v>
@@ -1783,7 +1782,7 @@
         <v>17</v>
       </c>
       <c r="D16" t="s" s="12">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="3"/>
@@ -1797,12 +1796,12 @@
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" t="s" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" t="s" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -1816,14 +1815,14 @@
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s" s="4">
         <v>44</v>
-      </c>
-      <c r="B18" t="s" s="4">
-        <v>45</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" t="s" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>

</xml_diff>